<commit_message>
Fix Resumo de publicados
</commit_message>
<xml_diff>
--- a/notebook/GEO/creditos/base_filtrada.xlsx
+++ b/notebook/GEO/creditos/base_filtrada.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R220"/>
+  <dimension ref="A1:R226"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11310,7 +11310,7 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>Sem Cobertura</t>
+          <t>Sem Cobertura - Atendido pela 1º NR</t>
         </is>
       </c>
       <c r="C177" t="inlineStr">
@@ -11364,7 +11364,7 @@
       </c>
       <c r="P177" t="inlineStr">
         <is>
-          <t>Fillipe Fernando - 27/05/2025 17:05:36</t>
+          <t>Fillipe Fernando - 28/05/2025 18:07:50</t>
         </is>
       </c>
       <c r="Q177" t="inlineStr"/>
@@ -11895,7 +11895,7 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>BLOCO 434066 - SEPLAG - Demais Orgãos</t>
+          <t>Análise - SEFAZ</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
@@ -11952,7 +11952,7 @@
       </c>
       <c r="P186" t="inlineStr">
         <is>
-          <t>Romero Cavalcanti - 19/05/2025 17:45:03</t>
+          <t>Romero Cavalcanti - 29/05/2025 14:04:46</t>
         </is>
       </c>
       <c r="Q186" t="inlineStr"/>
@@ -12418,7 +12418,7 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>Sem Cobertura</t>
+          <t>Sem Cobertura - Atendido pela 1º NR</t>
         </is>
       </c>
       <c r="C194" t="inlineStr">
@@ -12468,7 +12468,7 @@
       </c>
       <c r="P194" t="inlineStr">
         <is>
-          <t>Fillipe Fernando - 27/05/2025 17:05:36</t>
+          <t>Fillipe Fernando - 28/05/2025 18:09:34</t>
         </is>
       </c>
       <c r="Q194" t="inlineStr"/>
@@ -13569,7 +13569,7 @@
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>Análise - SOP</t>
+          <t>BLOCO 434050 - SOP - Superintendente</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
@@ -13626,7 +13626,11 @@
           <t>Fillipe Fernando - 26/05/2025 19:22:11</t>
         </is>
       </c>
-      <c r="P212" t="inlineStr"/>
+      <c r="P212" t="inlineStr">
+        <is>
+          <t>Isadora Costa - 29/05/2025 17:51:26</t>
+        </is>
+      </c>
       <c r="Q212" t="inlineStr"/>
       <c r="R212" t="inlineStr"/>
     </row>
@@ -13697,12 +13701,12 @@
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>BLOCO 434078 - SEFAZ - Despachos e Decretos</t>
+          <t>Publicado</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>Sem Cobertura</t>
+          <t>Sem Cobertura - Atendido pela 1º NR</t>
         </is>
       </c>
       <c r="C214" t="inlineStr">
@@ -13742,8 +13746,12 @@
       <c r="K214" s="2" t="n">
         <v>45798</v>
       </c>
-      <c r="L214" t="inlineStr"/>
-      <c r="M214" t="inlineStr"/>
+      <c r="L214" s="2" t="n">
+        <v>45806</v>
+      </c>
+      <c r="M214" t="n">
+        <v>102469</v>
+      </c>
       <c r="N214" t="inlineStr">
         <is>
           <t>SIM</t>
@@ -13756,7 +13764,7 @@
       </c>
       <c r="P214" t="inlineStr">
         <is>
-          <t>Fillipe Fernando - 28/05/2025 16:07:56</t>
+          <t>Felliphy Queiroz - 29/05/2025 12:01:01</t>
         </is>
       </c>
       <c r="Q214" t="inlineStr"/>
@@ -13830,7 +13838,7 @@
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>Excesso de Arrecadação</t>
+          <t>Redução/Anulação</t>
         </is>
       </c>
       <c r="C216" t="inlineStr">
@@ -13880,7 +13888,7 @@
       </c>
       <c r="P216" t="inlineStr">
         <is>
-          <t>Romero Cavalcanti - 28/05/2025 12:49:14</t>
+          <t>Isadora Costa - 29/05/2025 17:35:34</t>
         </is>
       </c>
       <c r="Q216" t="inlineStr"/>
@@ -13889,7 +13897,7 @@
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>Análise - SOP</t>
+          <t>BLOCO 434066 - SEPLAG - Demais Orgãos</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
@@ -13942,14 +13950,18 @@
           <t>Romero Cavalcanti - 28/05/2025 12:35:44</t>
         </is>
       </c>
-      <c r="P217" t="inlineStr"/>
+      <c r="P217" t="inlineStr">
+        <is>
+          <t>Isadora Costa - 29/05/2025 18:08:07</t>
+        </is>
+      </c>
       <c r="Q217" t="inlineStr"/>
       <c r="R217" t="inlineStr"/>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>Análise - SOP</t>
+          <t>BLOCO 434066 - SEPLAG - Demais Orgãos</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
@@ -14002,7 +14014,11 @@
           <t>Romero Cavalcanti - 28/05/2025 14:46:10</t>
         </is>
       </c>
-      <c r="P218" t="inlineStr"/>
+      <c r="P218" t="inlineStr">
+        <is>
+          <t>Isadora Costa - 29/05/2025 17:18:33</t>
+        </is>
+      </c>
       <c r="Q218" t="inlineStr"/>
       <c r="R218" t="inlineStr"/>
     </row>
@@ -14125,6 +14141,378 @@
       <c r="P220" t="inlineStr"/>
       <c r="Q220" t="inlineStr"/>
       <c r="R220" t="inlineStr"/>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr">
+        <is>
+          <t>Análise - SOP</t>
+        </is>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>Redução/Anulação</t>
+        </is>
+      </c>
+      <c r="C221" t="inlineStr">
+        <is>
+          <t>PMAL</t>
+        </is>
+      </c>
+      <c r="D221" t="inlineStr">
+        <is>
+          <t>E:01206.0000032071/2025</t>
+        </is>
+      </c>
+      <c r="E221" t="inlineStr">
+        <is>
+          <t>Suplementar</t>
+        </is>
+      </c>
+      <c r="F221" t="n">
+        <v>500</v>
+      </c>
+      <c r="G221" t="n">
+        <v>3</v>
+      </c>
+      <c r="H221" t="n">
+        <v>7838000</v>
+      </c>
+      <c r="I221" t="inlineStr">
+        <is>
+          <t>Complemento orçamentário para cumprir com as demandas inerentes a atividade Policial.</t>
+        </is>
+      </c>
+      <c r="J221" t="inlineStr"/>
+      <c r="K221" s="2" t="n">
+        <v>45805</v>
+      </c>
+      <c r="L221" t="inlineStr"/>
+      <c r="M221" t="inlineStr"/>
+      <c r="N221" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+      <c r="O221" t="inlineStr">
+        <is>
+          <t>Romero Cavalcanti - 28/05/2025 17:45:22</t>
+        </is>
+      </c>
+      <c r="P221" t="inlineStr"/>
+      <c r="Q221" t="inlineStr"/>
+      <c r="R221" t="inlineStr"/>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr">
+        <is>
+          <t>BLOCO 434078 - SEFAZ - Despachos e Decretos</t>
+        </is>
+      </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>Sem Cobertura - Atendido pela 1º NR</t>
+        </is>
+      </c>
+      <c r="C222" t="inlineStr">
+        <is>
+          <t>SECOM</t>
+        </is>
+      </c>
+      <c r="D222" t="inlineStr">
+        <is>
+          <t>E:01700.0000003990/2025</t>
+        </is>
+      </c>
+      <c r="E222" t="inlineStr">
+        <is>
+          <t>Suplementar</t>
+        </is>
+      </c>
+      <c r="F222" t="n">
+        <v>500</v>
+      </c>
+      <c r="G222" t="n">
+        <v>3</v>
+      </c>
+      <c r="H222" t="n">
+        <v>8155000</v>
+      </c>
+      <c r="I222" t="inlineStr">
+        <is>
+          <t>Atender a execução das atividades de publicidade planejadas para o primeiro bimestre de 2025.</t>
+        </is>
+      </c>
+      <c r="J222" t="inlineStr">
+        <is>
+          <t>ata 26</t>
+        </is>
+      </c>
+      <c r="K222" s="2" t="n">
+        <v>45805</v>
+      </c>
+      <c r="L222" t="inlineStr"/>
+      <c r="M222" t="inlineStr"/>
+      <c r="N222" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+      <c r="O222" t="inlineStr">
+        <is>
+          <t>Fillipe Fernando - 28/05/2025 18:03:33</t>
+        </is>
+      </c>
+      <c r="P222" t="inlineStr">
+        <is>
+          <t>Fillipe Fernando - 28/05/2025 20:48:39</t>
+        </is>
+      </c>
+      <c r="Q222" t="inlineStr"/>
+      <c r="R222" t="inlineStr"/>
+    </row>
+    <row r="223">
+      <c r="A223" t="inlineStr">
+        <is>
+          <t>Análise - CPOF</t>
+        </is>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>Sem Cobertura</t>
+        </is>
+      </c>
+      <c r="C223" t="inlineStr">
+        <is>
+          <t>SECOM</t>
+        </is>
+      </c>
+      <c r="D223" t="inlineStr">
+        <is>
+          <t>E:02200.0000000671/2025</t>
+        </is>
+      </c>
+      <c r="E223" t="inlineStr">
+        <is>
+          <t>Suplementar</t>
+        </is>
+      </c>
+      <c r="F223" t="n">
+        <v>500</v>
+      </c>
+      <c r="G223" t="n">
+        <v>3</v>
+      </c>
+      <c r="H223" t="n">
+        <v>12700000</v>
+      </c>
+      <c r="I223" t="inlineStr">
+        <is>
+          <t>Atender a ações previstas para os meses de junho e julho do 2025.</t>
+        </is>
+      </c>
+      <c r="J223" t="inlineStr"/>
+      <c r="K223" s="2" t="n">
+        <v>45806</v>
+      </c>
+      <c r="L223" t="inlineStr"/>
+      <c r="M223" t="inlineStr"/>
+      <c r="N223" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+      <c r="O223" t="inlineStr">
+        <is>
+          <t>Fillipe Fernando - 29/05/2025 13:12:08</t>
+        </is>
+      </c>
+      <c r="P223" t="inlineStr">
+        <is>
+          <t>Romero Cavalcanti - 29/05/2025 17:56:26</t>
+        </is>
+      </c>
+      <c r="Q223" t="inlineStr"/>
+      <c r="R223" t="inlineStr"/>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr">
+        <is>
+          <t>Análise - SOP</t>
+        </is>
+      </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>Sem Cobertura</t>
+        </is>
+      </c>
+      <c r="C224" t="inlineStr">
+        <is>
+          <t>SETRAND</t>
+        </is>
+      </c>
+      <c r="D224" t="inlineStr">
+        <is>
+          <t>E:35032.0000001392/2025</t>
+        </is>
+      </c>
+      <c r="E224" t="inlineStr">
+        <is>
+          <t>Suplementar</t>
+        </is>
+      </c>
+      <c r="F224" t="n">
+        <v>754</v>
+      </c>
+      <c r="G224" t="n">
+        <v>4</v>
+      </c>
+      <c r="H224" t="n">
+        <v>8313500</v>
+      </c>
+      <c r="I224" t="inlineStr">
+        <is>
+          <t>DUPLICAÇÃO, RESTAURAÇÃO COM MELHORIAS DA RODOVIA AL 101 NORTE, TRECHO: MACEIÓ/BARRA DE SANTO ANTÔNIO</t>
+        </is>
+      </c>
+      <c r="J224" t="inlineStr"/>
+      <c r="K224" s="2" t="n">
+        <v>45807</v>
+      </c>
+      <c r="L224" t="inlineStr"/>
+      <c r="M224" t="inlineStr"/>
+      <c r="N224" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+      <c r="O224" t="inlineStr">
+        <is>
+          <t>Fillipe Fernando - 30/05/2025 16:00:12</t>
+        </is>
+      </c>
+      <c r="P224" t="inlineStr"/>
+      <c r="Q224" t="inlineStr"/>
+      <c r="R224" t="inlineStr"/>
+    </row>
+    <row r="225">
+      <c r="A225" t="inlineStr">
+        <is>
+          <t>Análise - SOP</t>
+        </is>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>Redução/Anulação</t>
+        </is>
+      </c>
+      <c r="C225" t="inlineStr">
+        <is>
+          <t>FUNTURIS</t>
+        </is>
+      </c>
+      <c r="D225" t="inlineStr">
+        <is>
+          <t>E:29032.0000000514/2025</t>
+        </is>
+      </c>
+      <c r="E225" t="inlineStr">
+        <is>
+          <t>Suplementar</t>
+        </is>
+      </c>
+      <c r="F225" t="n">
+        <v>759</v>
+      </c>
+      <c r="G225" t="n">
+        <v>3</v>
+      </c>
+      <c r="H225" t="n">
+        <v>400000</v>
+      </c>
+      <c r="I225" t="inlineStr">
+        <is>
+          <t>Ampliação e consolidação do destino Alagoas nos mercados Nacional e Internacional do Fundo do Turismo – FUNTURIS da Secretaria de Estado do Turismo - SETUR.</t>
+        </is>
+      </c>
+      <c r="J225" t="inlineStr"/>
+      <c r="K225" s="2" t="n">
+        <v>45807</v>
+      </c>
+      <c r="L225" t="inlineStr"/>
+      <c r="M225" t="inlineStr"/>
+      <c r="N225" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+      <c r="O225" t="inlineStr">
+        <is>
+          <t>Fillipe Fernando - 30/05/2025 16:03:58</t>
+        </is>
+      </c>
+      <c r="P225" t="inlineStr"/>
+      <c r="Q225" t="inlineStr"/>
+      <c r="R225" t="inlineStr"/>
+    </row>
+    <row r="226">
+      <c r="A226" t="inlineStr">
+        <is>
+          <t>Análise - SOP</t>
+        </is>
+      </c>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>Sem Cobertura</t>
+        </is>
+      </c>
+      <c r="C226" t="inlineStr">
+        <is>
+          <t>SETUR</t>
+        </is>
+      </c>
+      <c r="D226" t="inlineStr">
+        <is>
+          <t>E:29032.0000000509/2025</t>
+        </is>
+      </c>
+      <c r="E226" t="inlineStr">
+        <is>
+          <t>Suplementar</t>
+        </is>
+      </c>
+      <c r="F226" t="n">
+        <v>500</v>
+      </c>
+      <c r="G226" t="n">
+        <v>3</v>
+      </c>
+      <c r="H226" t="n">
+        <v>4813155.82</v>
+      </c>
+      <c r="I226" t="inlineStr">
+        <is>
+          <t>Atender a diversos contratos de manutenção e eventos.</t>
+        </is>
+      </c>
+      <c r="J226" t="inlineStr"/>
+      <c r="K226" s="2" t="n">
+        <v>45807</v>
+      </c>
+      <c r="L226" t="inlineStr"/>
+      <c r="M226" t="inlineStr"/>
+      <c r="N226" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+      <c r="O226" t="inlineStr">
+        <is>
+          <t>Fillipe Fernando - 30/05/2025 16:07:28</t>
+        </is>
+      </c>
+      <c r="P226" t="inlineStr"/>
+      <c r="Q226" t="inlineStr"/>
+      <c r="R226" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>